<commit_message>
Updated the UI to show selected state's image and the graph connector in the map
</commit_message>
<xml_diff>
--- a/city_list.xlsx
+++ b/city_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/nich7312_colorado_edu/Documents/01. Study/03. CUB Courses/01. Undergoing Courses/Data Structures/04. Project/Shortest Path Map/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/nich7312_colorado_edu/Documents/01. Study/03. CUB Courses/01. Undergoing Courses/Data Structures/04. Project/Repo/Dynamic_Shortest_Path/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_F25DC773A252ABDACC104850E9DC4B225BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{324592CB-7105-49E7-8172-63E4A7C1C84D}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="11_F25DC773A252ABDACC104850E9DC4B225BDE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53F7DF8B-76CC-43B7-9405-A6EE4601D10C}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="420" windowWidth="16200" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,24 +51,9 @@
     <t>Fort Collins</t>
   </si>
   <si>
-    <t>Lakewood</t>
-  </si>
-  <si>
-    <t>Thornton</t>
-  </si>
-  <si>
-    <t>Arvada</t>
-  </si>
-  <si>
     <t>Boulder</t>
   </si>
   <si>
-    <t>Westminster</t>
-  </si>
-  <si>
-    <t>Centennial</t>
-  </si>
-  <si>
     <t>California</t>
   </si>
   <si>
@@ -90,49 +75,64 @@
     <t>Sacramento</t>
   </si>
   <si>
-    <t>Long Beach</t>
-  </si>
-  <si>
     <t>Oakland</t>
   </si>
   <si>
-    <t>Riverside</t>
-  </si>
-  <si>
-    <t>Irvine</t>
-  </si>
-  <si>
     <t>New York</t>
   </si>
   <si>
     <t>New York City</t>
   </si>
   <si>
-    <t>Hempstead</t>
-  </si>
-  <si>
     <t>Brookhaven</t>
   </si>
   <si>
-    <t>Islip</t>
-  </si>
-  <si>
     <t>Buffalo</t>
   </si>
   <si>
-    <t>Oyster Bay</t>
-  </si>
-  <si>
-    <t>Babylon</t>
-  </si>
-  <si>
     <t>Rochester</t>
   </si>
   <si>
     <t>Syracuse</t>
   </si>
   <si>
-    <t>Yonkers</t>
+    <t>Aspen</t>
+  </si>
+  <si>
+    <t>Burlington</t>
+  </si>
+  <si>
+    <t>Gunnison</t>
+  </si>
+  <si>
+    <t>Durango</t>
+  </si>
+  <si>
+    <t>Springfield</t>
+  </si>
+  <si>
+    <t>Dunkirk</t>
+  </si>
+  <si>
+    <t>Watertown</t>
+  </si>
+  <si>
+    <t>Binghamton</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>Kingston</t>
+  </si>
+  <si>
+    <t>Redding</t>
+  </si>
+  <si>
+    <t>Eureka</t>
+  </si>
+  <si>
+    <t>Santa Barbara</t>
   </si>
 </sst>
 </file>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -517,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -533,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -541,7 +541,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -549,7 +549,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -557,116 +557,116 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
         <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
@@ -674,50 +674,50 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>